<commit_message>
Plot summary for z-scores
- plot summary for Z1 - Z4 ( z-scores )
- 4 different plots
</commit_message>
<xml_diff>
--- a/raw_data_diesel.xlsx
+++ b/raw_data_diesel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akmor\Downloads\traction_motor-main\traction_motor-main\ken_python_traction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB720E0-8201-4B04-B79C-8227D15DFECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21A5E23-2C07-48CB-8E0B-F74DD021DC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="3552" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>MPH</t>
   </si>
@@ -75,6 +75,21 @@
   </si>
   <si>
     <t>INDEX_TR2</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Z2</t>
+  </si>
+  <si>
+    <t>Z3</t>
+  </si>
+  <si>
+    <t>Z4</t>
   </si>
 </sst>
 </file>
@@ -423,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,12 +450,11 @@
     <col min="2" max="4" width="10.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.21875" style="3" customWidth="1"/>
     <col min="6" max="13" width="8.88671875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1"/>
-    <col min="15" max="15" width="8.88671875" style="4"/>
-    <col min="16" max="16384" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="8.88671875" style="4"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,25 +494,36 @@
       <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>5</v>
       </c>
       <c r="B2" s="3">
-        <f t="shared" ref="B2:B9" si="0">F2/M2</f>
-        <v>0.98701298701298701</v>
+        <v>1.04</v>
       </c>
       <c r="C2" s="3">
-        <f t="shared" ref="C2:C9" si="1">G2/M2</f>
+        <f t="shared" ref="C2:C9" si="0">G2/M2</f>
         <v>1.0389610389610389</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D9" si="2">H2/M2</f>
+        <f t="shared" ref="D2:D9" si="1">H2/M2</f>
         <v>0.93506493506493504</v>
       </c>
       <c r="E2" s="3">
-        <f t="shared" ref="E2:E9" si="3">I2/M2</f>
+        <f t="shared" ref="E2:E9" si="2">I2/M2</f>
         <v>1.0389610389610389</v>
       </c>
       <c r="F2" s="1">
@@ -525,25 +550,41 @@
       <c r="M2" s="1">
         <v>962.5</v>
       </c>
+      <c r="N2" s="4">
+        <f>(F2-M2)/L2</f>
+        <v>-0.30149541726965751</v>
+      </c>
+      <c r="O2" s="4">
+        <f>(G2-M2)/L2</f>
+        <v>0.90448625180897246</v>
+      </c>
+      <c r="P2" s="4">
+        <f>(H2-M2)/L2</f>
+        <v>-1.5074770863482874</v>
+      </c>
+      <c r="Q2" s="4">
+        <f>(I2-M2)/L2</f>
+        <v>0.90448625180897246</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>15</v>
       </c>
       <c r="B3" s="3">
+        <f t="shared" ref="B3:B9" si="3">F3/M3</f>
+        <v>0.96644295302013428</v>
+      </c>
+      <c r="C3" s="3">
         <f t="shared" si="0"/>
         <v>0.96644295302013428</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <f t="shared" si="1"/>
-        <v>0.96644295302013428</v>
-      </c>
-      <c r="D3" s="3">
+        <v>1.0201342281879195</v>
+      </c>
+      <c r="E3" s="3">
         <f t="shared" si="2"/>
-        <v>1.0201342281879195</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" si="3"/>
         <v>1.0469798657718121</v>
       </c>
       <c r="F3" s="1">
@@ -570,27 +611,43 @@
       <c r="M3" s="1">
         <v>931.25</v>
       </c>
+      <c r="N3" s="4">
+        <f t="shared" ref="N3:N9" si="4">(F3-M3)/L3</f>
+        <v>-0.96213054187192126</v>
+      </c>
+      <c r="O3" s="4">
+        <f t="shared" ref="O3:O9" si="5">(G3-M3)/L3</f>
+        <v>-0.96213054187192126</v>
+      </c>
+      <c r="P3" s="4">
+        <f t="shared" ref="P3:P9" si="6">(H3-M3)/L3</f>
+        <v>0.5772783251231528</v>
+      </c>
+      <c r="Q3" s="4">
+        <f t="shared" ref="Q3:Q9" si="7">(I3-M3)/L3</f>
+        <v>1.3469827586206897</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>25</v>
       </c>
       <c r="B4" s="3">
+        <f t="shared" si="3"/>
+        <v>0.96969696969696972</v>
+      </c>
+      <c r="C4" s="3">
         <f t="shared" si="0"/>
         <v>0.96969696969696972</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <f t="shared" si="1"/>
-        <v>0.96969696969696972</v>
-      </c>
-      <c r="D4" s="3">
+        <v>1.0303030303030303</v>
+      </c>
+      <c r="E4" s="3">
         <f t="shared" si="2"/>
         <v>1.0303030303030303</v>
       </c>
-      <c r="E4" s="3">
-        <f t="shared" si="3"/>
-        <v>1.0303030303030303</v>
-      </c>
       <c r="F4" s="1">
         <v>800</v>
       </c>
@@ -615,25 +672,41 @@
       <c r="M4" s="1">
         <v>825</v>
       </c>
+      <c r="N4" s="4">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="P4" s="4">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>35</v>
       </c>
       <c r="B5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.9375</v>
+      </c>
+      <c r="C5" s="3">
         <f t="shared" si="0"/>
+        <v>1.125</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="1"/>
         <v>0.9375</v>
       </c>
-      <c r="C5" s="3">
-        <f t="shared" si="1"/>
-        <v>1.125</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <f t="shared" si="2"/>
-        <v>0.9375</v>
-      </c>
-      <c r="E5" s="3">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F5" s="1">
@@ -660,25 +733,41 @@
       <c r="M5" s="1">
         <v>800</v>
       </c>
+      <c r="N5" s="4">
+        <f t="shared" si="4"/>
+        <v>-0.81645983017635526</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="5"/>
+        <v>1.6329196603527105</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.81645983017635526</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45</v>
       </c>
       <c r="B6" s="3">
+        <f t="shared" si="3"/>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>0.81632653061224492</v>
-      </c>
-      <c r="C6" s="3">
+        <v>1.0204081632653061</v>
+      </c>
+      <c r="D6" s="3">
         <f t="shared" si="1"/>
-        <v>1.0204081632653061</v>
-      </c>
-      <c r="D6" s="3">
+        <v>0.93877551020408168</v>
+      </c>
+      <c r="E6" s="3">
         <f t="shared" si="2"/>
-        <v>0.93877551020408168</v>
-      </c>
-      <c r="E6" s="3">
-        <f t="shared" si="3"/>
         <v>1.2244897959183674</v>
       </c>
       <c r="F6" s="1">
@@ -705,25 +794,41 @@
       <c r="M6" s="1">
         <v>735</v>
       </c>
+      <c r="N6" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.2362637362637363</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="5"/>
+        <v>0.13736263736263735</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.41208791208791207</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" si="7"/>
+        <v>1.5109890109890109</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>55</v>
       </c>
       <c r="B7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.85106382978723405</v>
+      </c>
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
-        <v>0.85106382978723405</v>
-      </c>
-      <c r="C7" s="3">
+        <v>1.0212765957446808</v>
+      </c>
+      <c r="D7" s="3">
         <f t="shared" si="1"/>
-        <v>1.0212765957446808</v>
-      </c>
-      <c r="D7" s="3">
+        <v>0.93617021276595747</v>
+      </c>
+      <c r="E7" s="3">
         <f t="shared" si="2"/>
-        <v>0.93617021276595747</v>
-      </c>
-      <c r="E7" s="3">
-        <f t="shared" si="3"/>
         <v>1.1914893617021276</v>
       </c>
       <c r="F7" s="1">
@@ -750,25 +855,41 @@
       <c r="M7" s="1">
         <v>587.5</v>
       </c>
+      <c r="N7" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.1832319134550371</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="5"/>
+        <v>0.16903313049357674</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.50709939148073024</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="7"/>
+        <v>1.5212981744421905</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>65</v>
       </c>
       <c r="B8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.89411764705882357</v>
+      </c>
+      <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>0.89411764705882357</v>
-      </c>
-      <c r="C8" s="3">
+        <v>1.0352941176470589</v>
+      </c>
+      <c r="D8" s="3">
         <f t="shared" si="1"/>
-        <v>1.0352941176470589</v>
-      </c>
-      <c r="D8" s="3">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="E8" s="3">
         <f t="shared" si="2"/>
-        <v>0.94117647058823528</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="3"/>
         <v>1.1294117647058823</v>
       </c>
       <c r="F8" s="1">
@@ -795,25 +916,41 @@
       <c r="M8" s="1">
         <v>531.25</v>
       </c>
+      <c r="N8" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.1716309102270361</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="5"/>
+        <v>0.39054363674234538</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="6"/>
+        <v>-0.65090606123724226</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" si="7"/>
+        <v>1.4319933347219329</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>75</v>
       </c>
       <c r="B9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.87671232876712324</v>
+      </c>
+      <c r="C9" s="3">
         <f t="shared" si="0"/>
-        <v>0.87671232876712324</v>
-      </c>
-      <c r="C9" s="3">
+        <v>0.98630136986301364</v>
+      </c>
+      <c r="D9" s="3">
         <f t="shared" si="1"/>
-        <v>0.98630136986301364</v>
-      </c>
-      <c r="D9" s="3">
+        <v>1.0410958904109588</v>
+      </c>
+      <c r="E9" s="3">
         <f t="shared" si="2"/>
-        <v>1.0410958904109588</v>
-      </c>
-      <c r="E9" s="3">
-        <f t="shared" si="3"/>
         <v>1.095890410958904</v>
       </c>
       <c r="F9" s="1">
@@ -839,6 +976,27 @@
       </c>
       <c r="M9" s="1">
         <v>456.25</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="4"/>
+        <v>-1.5210924824229315</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.16901027582477016</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="6"/>
+        <v>0.5070308274743105</v>
+      </c>
+      <c r="Q9" s="4">
+        <f t="shared" si="7"/>
+        <v>1.183071930773391</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K15" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>